<commit_message>
Improved logging and test data.
</commit_message>
<xml_diff>
--- a/tests/sample_files/sampleEntityDictionary.xlsx
+++ b/tests/sample_files/sampleEntityDictionary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_tool\tests\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_entities\tests\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8550" windowWidth="20400" windowHeight="10410"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="20400" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>pattern</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>TOMES_PATTERN: {"A","B"}, {"1","2"}</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"A","B"}, {1,"2"}</t>
+  </si>
+  <si>
+    <t>Should yield 4 (2*2) manifestations AFTER first bing unable to sort due to the "1" not being in quotes.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +175,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -563,11 +602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,54 +720,83 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B1048576 B1 B4">
-    <cfRule type="duplicateValues" dxfId="11" priority="22"/>
-    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="[">
+  <conditionalFormatting sqref="B8:B1048576 B1 B4">
+    <cfRule type="duplicateValues" dxfId="14" priority="25"/>
+    <cfRule type="containsText" dxfId="13" priority="26" operator="containsText" text="[">
       <formula>NOT(ISERROR(SEARCH("[",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="24" operator="containsText" text=".txt">
+    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text=".txt">
       <formula>NOT(ISERROR(SEARCH(".txt",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="[">
+      <formula>NOT(ISERROR(SEARCH("[",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text=".txt">
+      <formula>NOT(ISERROR(SEARCH(".txt",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
     <cfRule type="duplicateValues" dxfId="8" priority="10"/>
     <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="[">
-      <formula>NOT(ISERROR(SEARCH("[",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("[",B3)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text=".txt">
-      <formula>NOT(ISERROR(SEARCH(".txt",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH(".txt",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="B5">
     <cfRule type="duplicateValues" dxfId="5" priority="7"/>
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="[">
-      <formula>NOT(ISERROR(SEARCH("[",B3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("[",B5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text=".txt">
-      <formula>NOT(ISERROR(SEARCH(".txt",B3)))</formula>
+      <formula>NOT(ISERROR(SEARCH(".txt",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="[">
-      <formula>NOT(ISERROR(SEARCH("[",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text=".txt">
-      <formula>NOT(ISERROR(SEARCH(".txt",B5)))</formula>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="[">
+      <formula>NOT(ISERROR(SEARCH("[",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text=".txt">
+      <formula>NOT(ISERROR(SEARCH(".txt",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed bug re: Linux vs Windows sorting.
</commit_message>
<xml_diff>
--- a/tests/sample_files/sampleEntityDictionary.xlsx
+++ b/tests/sample_files/sampleEntityDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_entities\tests\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6FB4F16D-68DB-4D55-B777-7D4DD63C9FDF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6756B18D-C090-4A38-8BB4-C958113AB97A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9900" windowWidth="20400" windowHeight="10410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="20400" windowHeight="10410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="3" r:id="rId1"/>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>